<commit_message>
Fix: skip Excel temp files, add gitignore patterns
</commit_message>
<xml_diff>
--- a/data/Robotics_Companies_Careers.xlsx
+++ b/data/Robotics_Companies_Careers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham09\Documents\job-search-agent\job-search-agent\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham09\Downloads\git repo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BCE72F-A768-4108-BF60-A2F9FD906109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E27F21F-8993-42A9-9C70-E14D1D7D4E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Robotics Companies" sheetId="1" r:id="rId1"/>
@@ -1052,8 +1052,8 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="A25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix for some different links
</commit_message>
<xml_diff>
--- a/data/Robotics_Companies_Careers.xlsx
+++ b/data/Robotics_Companies_Careers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham09\Downloads\git repo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F223F0A7-0CB1-467D-A418-7E30A92DB5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B71D4C0-651E-43E8-97C2-BE9D4358783D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Robotics Companies" sheetId="1" r:id="rId1"/>
@@ -1072,8 +1072,8 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>